<commit_message>
file processor api working without sendin email/wp messages
</commit_message>
<xml_diff>
--- a/Transactions case study.xlsx
+++ b/Transactions case study.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\Desktop\Simetrik\People\Hiring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MichaelGY\Documents\GitHub\simetrik-case-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F07F1A74-3B97-46F2-9A4E-80E15103A770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6A10DA-7193-45FD-AA1C-5A0C4ADF4C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -397,19 +397,19 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.36328125" customWidth="1"/>
-    <col min="7" max="7" width="29.6328125" customWidth="1"/>
-    <col min="8" max="8" width="20.26953125" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" customWidth="1"/>
-    <col min="10" max="10" width="23.6328125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -471,7 +471,7 @@
       </c>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -501,7 +501,7 @@
       </c>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -531,7 +531,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -561,7 +561,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>44321</v>
       </c>
@@ -591,7 +591,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -620,7 +620,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -649,7 +649,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -678,7 +678,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -707,7 +707,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>44321</v>
       </c>
@@ -736,7 +736,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -765,7 +765,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -794,7 +794,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -823,7 +823,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>44321.337002314816</v>
       </c>
@@ -852,7 +852,7 @@
         <v>5556400945</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>44321</v>
       </c>
@@ -883,5 +883,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>